<commit_message>
ajeste detalles y valores en box
</commit_message>
<xml_diff>
--- a/app-medicine-r/modulos/data/datos_suspensiones_sankey_bd.xlsx
+++ b/app-medicine-r/modulos/data/datos_suspensiones_sankey_bd.xlsx
@@ -1,26 +1,39 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\documentos juan\Salud\app_health_r_medicine\app-mvp\modulos\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\rstudio\app_health_r_medicine\app-medicine-r\modulos\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B24E7024-E4B5-438F-948B-5318EDC18E8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA2A6FB8-B9B1-43BC-B2E3-859309F1042F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33000" yWindow="1755" windowWidth="21600" windowHeight="11235" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="39">
   <si>
     <t>source</t>
   </si>
@@ -134,6 +147,9 @@
   </si>
   <si>
     <t>Emergencia sanitaria COVID-19: Resguardo de usuarios y personal de salud</t>
+  </si>
+  <si>
+    <t>porcentaje</t>
   </si>
 </sst>
 </file>
@@ -157,7 +173,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -165,12 +181,22 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -189,7 +215,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -485,29 +511,33 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C36"/>
+  <dimension ref="A1:D36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="A36" sqref="A1:A36"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="66.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D1" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -517,8 +547,12 @@
       <c r="C2">
         <v>279</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D2">
+        <f>C2/SUM($C$2:$C$6)</f>
+        <v>0.48186528497409326</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -528,8 +562,12 @@
       <c r="C3">
         <v>140</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D3">
+        <f t="shared" ref="D3:D6" si="0">C3/SUM($C$2:$C$6)</f>
+        <v>0.24179620034542315</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -539,8 +577,12 @@
       <c r="C4">
         <v>65</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D4">
+        <f t="shared" si="0"/>
+        <v>0.11226252158894647</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -550,19 +592,27 @@
       <c r="C5">
         <v>42</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+      <c r="D5">
+        <f t="shared" si="0"/>
+        <v>7.2538860103626937E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="1">
         <v>53</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D6" s="1">
+        <f t="shared" si="0"/>
+        <v>9.1537132987910191E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -572,8 +622,12 @@
       <c r="C7">
         <v>62</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D7">
+        <f>C7/SUM($C$7:$C$36)</f>
+        <v>0.10708117443868739</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>4</v>
       </c>
@@ -583,8 +637,12 @@
       <c r="C8">
         <v>56</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D8">
+        <f t="shared" ref="D8:D36" si="1">C8/SUM($C$7:$C$36)</f>
+        <v>9.6718480138169263E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>4</v>
       </c>
@@ -594,8 +652,12 @@
       <c r="C9">
         <v>18</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D9">
+        <f t="shared" si="1"/>
+        <v>3.1088082901554404E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>4</v>
       </c>
@@ -605,8 +667,12 @@
       <c r="C10">
         <v>22</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D10">
+        <f t="shared" si="1"/>
+        <v>3.7996545768566495E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>4</v>
       </c>
@@ -616,8 +682,12 @@
       <c r="C11">
         <v>16</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D11">
+        <f t="shared" si="1"/>
+        <v>2.7633851468048358E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>4</v>
       </c>
@@ -627,8 +697,12 @@
       <c r="C12">
         <v>19</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D12">
+        <f t="shared" si="1"/>
+        <v>3.281519861830743E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>4</v>
       </c>
@@ -638,8 +712,12 @@
       <c r="C13">
         <v>13</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D13">
+        <f t="shared" si="1"/>
+        <v>2.2452504317789293E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>4</v>
       </c>
@@ -649,8 +727,12 @@
       <c r="C14">
         <v>20</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D14">
+        <f t="shared" si="1"/>
+        <v>3.4542314335060449E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>4</v>
       </c>
@@ -660,8 +742,12 @@
       <c r="C15">
         <v>18</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D15">
+        <f t="shared" si="1"/>
+        <v>3.1088082901554404E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>4</v>
       </c>
@@ -671,8 +757,12 @@
       <c r="C16">
         <v>9</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D16">
+        <f t="shared" si="1"/>
+        <v>1.5544041450777202E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>4</v>
       </c>
@@ -682,8 +772,12 @@
       <c r="C17">
         <v>11</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D17">
+        <f t="shared" si="1"/>
+        <v>1.8998272884283247E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>4</v>
       </c>
@@ -693,8 +787,12 @@
       <c r="C18">
         <v>7</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D18">
+        <f t="shared" si="1"/>
+        <v>1.2089810017271158E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>4</v>
       </c>
@@ -704,8 +802,12 @@
       <c r="C19">
         <v>4</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D19">
+        <f t="shared" si="1"/>
+        <v>6.9084628670120895E-3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>4</v>
       </c>
@@ -715,8 +817,12 @@
       <c r="C20">
         <v>2</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D20">
+        <f t="shared" si="1"/>
+        <v>3.4542314335060447E-3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>4</v>
       </c>
@@ -726,8 +832,12 @@
       <c r="C21">
         <v>1</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D21">
+        <f t="shared" si="1"/>
+        <v>1.7271157167530224E-3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>4</v>
       </c>
@@ -737,8 +847,12 @@
       <c r="C22">
         <v>1</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D22">
+        <f t="shared" si="1"/>
+        <v>1.7271157167530224E-3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>5</v>
       </c>
@@ -748,8 +862,12 @@
       <c r="C23">
         <v>89</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D23">
+        <f t="shared" si="1"/>
+        <v>0.153713298791019</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>5</v>
       </c>
@@ -759,8 +877,12 @@
       <c r="C24">
         <v>28</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D24">
+        <f t="shared" si="1"/>
+        <v>4.8359240069084632E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>5</v>
       </c>
@@ -770,8 +892,12 @@
       <c r="C25">
         <v>18</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D25">
+        <f t="shared" si="1"/>
+        <v>3.1088082901554404E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>5</v>
       </c>
@@ -781,8 +907,12 @@
       <c r="C26">
         <v>5</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D26">
+        <f t="shared" si="1"/>
+        <v>8.6355785837651123E-3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>6</v>
       </c>
@@ -792,8 +922,12 @@
       <c r="C27">
         <v>24</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D27">
+        <f t="shared" si="1"/>
+        <v>4.145077720207254E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>6</v>
       </c>
@@ -803,8 +937,12 @@
       <c r="C28">
         <v>32</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D28">
+        <f t="shared" si="1"/>
+        <v>5.5267702936096716E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>6</v>
       </c>
@@ -814,8 +952,12 @@
       <c r="C29">
         <v>7</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D29">
+        <f t="shared" si="1"/>
+        <v>1.2089810017271158E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>6</v>
       </c>
@@ -825,8 +967,12 @@
       <c r="C30">
         <v>2</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D30">
+        <f t="shared" si="1"/>
+        <v>3.4542314335060447E-3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>7</v>
       </c>
@@ -836,8 +982,12 @@
       <c r="C31">
         <v>20</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D31">
+        <f t="shared" si="1"/>
+        <v>3.4542314335060449E-2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>7</v>
       </c>
@@ -847,8 +997,12 @@
       <c r="C32">
         <v>11</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D32">
+        <f t="shared" si="1"/>
+        <v>1.8998272884283247E-2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>7</v>
       </c>
@@ -858,8 +1012,12 @@
       <c r="C33">
         <v>8</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D33">
+        <f t="shared" si="1"/>
+        <v>1.3816925734024179E-2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>7</v>
       </c>
@@ -869,8 +1027,12 @@
       <c r="C34">
         <v>2</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D34">
+        <f t="shared" si="1"/>
+        <v>3.4542314335060447E-3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>7</v>
       </c>
@@ -880,8 +1042,12 @@
       <c r="C35">
         <v>1</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D35">
+        <f t="shared" si="1"/>
+        <v>1.7271157167530224E-3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>8</v>
       </c>
@@ -890,6 +1056,10 @@
       </c>
       <c r="C36">
         <v>53</v>
+      </c>
+      <c r="D36">
+        <f t="shared" si="1"/>
+        <v>9.1537132987910191E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>